<commit_message>
Added some instructions to the excel sheet.
</commit_message>
<xml_diff>
--- a/Expedia_automation/Data_sheets/Data_sheets_expedia.xlsx
+++ b/Expedia_automation/Data_sheets/Data_sheets_expedia.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Selenium\Selenium projects\Expedia_automation\Data_sheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E08E5643-6BB5-44A4-8D72-793192AA5D9B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7992DB3-2AD1-4F77-8CF5-C99A8A47A01F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FlightsOnlyPositive" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="31">
   <si>
     <t>One-way</t>
   </si>
@@ -47,18 +47,12 @@
     <t>Departure Date (in dd/mm/yyyy)</t>
   </si>
   <si>
-    <t>Hyderabad</t>
-  </si>
-  <si>
     <t>12/01/2020</t>
   </si>
   <si>
     <t>Hotel Check-in Date (in dd/mm/yyyy)</t>
   </si>
   <si>
-    <t>New Delhi</t>
-  </si>
-  <si>
     <t>Chennai</t>
   </si>
   <si>
@@ -98,14 +92,36 @@
     <t>Trivandrum</t>
   </si>
   <si>
-    <t>09/11/2019</t>
+    <t>18/12/2019</t>
+  </si>
+  <si>
+    <t>new york</t>
+  </si>
+  <si>
+    <t>hyderabad</t>
+  </si>
+  <si>
+    <t>mumbai</t>
+  </si>
+  <si>
+    <t>delhi</t>
+  </si>
+  <si>
+    <t>Delhi</t>
+  </si>
+  <si>
+    <t>09/01/2020</t>
+  </si>
+  <si>
+    <t>Instruction - Put the start tag (One-way) before the first column and the first row to be used and the end tag (One-way) after the last column and last row to be used.
+Only use future dates here.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -124,6 +140,16 @@
     <font>
       <sz val="11"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -146,7 +172,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -154,7 +180,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -370,9 +399,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E1000"/>
+  <dimension ref="A1:H1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
@@ -380,10 +409,13 @@
     <col min="2" max="2" width="12.6640625" customWidth="1"/>
     <col min="3" max="3" width="15.6640625" customWidth="1"/>
     <col min="4" max="4" width="24.5" customWidth="1"/>
-    <col min="5" max="26" width="7.6640625" customWidth="1"/>
+    <col min="5" max="6" width="7.6640625" customWidth="1"/>
+    <col min="7" max="7" width="24.4140625" customWidth="1"/>
+    <col min="8" max="8" width="26.33203125" customWidth="1"/>
+    <col min="9" max="26" width="7.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -397,9 +429,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B2" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>5</v>
@@ -408,64 +440,72 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B4" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>9</v>
-      </c>
     </row>
-    <row r="4" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>14</v>
+    <row r="6" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B6" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D6" s="6" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E7" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="9" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="10" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="11" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="12" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="13" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="14" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="15" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="16" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="8" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="9" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="10" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="11" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="12" spans="1:8" ht="31.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G12" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="H12" s="8"/>
+    </row>
+    <row r="13" spans="1:8" ht="46" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G13" s="8"/>
+      <c r="H13" s="8"/>
+    </row>
+    <row r="14" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="15" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="16" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="17" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="18" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1451,6 +1491,9 @@
     <row r="999" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="1000" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="G12:H13"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="portrait"/>
 </worksheet>
@@ -1461,20 +1504,20 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:J12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="4" max="4" width="31.4140625" customWidth="1"/>
     <col min="5" max="5" width="29" customWidth="1"/>
     <col min="6" max="6" width="28.6640625" customWidth="1"/>
+    <col min="9" max="9" width="19.83203125" customWidth="1"/>
+    <col min="10" max="10" width="18.9140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
@@ -1488,52 +1531,84 @@
         <v>7</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F1" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="B2" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>13</v>
       </c>
+      <c r="D2" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>16</v>
+      </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="B2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" ht="14.5" x14ac:dyDescent="0.35">
       <c r="B3" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="F3" s="7">
-        <v>43817</v>
+        <v>14</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="G4" s="2" t="s">
+    <row r="4" spans="1:10" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="B4" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="G5" s="2" t="s">
         <v>1</v>
       </c>
+    </row>
+    <row r="11" spans="1:10" ht="49.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="I11" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="J11" s="8"/>
+    </row>
+    <row r="12" spans="1:10" ht="34" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="I12" s="8"/>
+      <c r="J12" s="8"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="I11:J12"/>
+  </mergeCells>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Developed automation code aligned towards Test Driven Development (TDD) and Page Object Model (POM) practices. More changes to come.
</commit_message>
<xml_diff>
--- a/Expedia_automation/Data_sheets/Data_sheets_expedia.xlsx
+++ b/Expedia_automation/Data_sheets/Data_sheets_expedia.xlsx
@@ -1,27 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Selenium\Selenium projects\Expedia_automation\Data_sheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7992DB3-2AD1-4F77-8CF5-C99A8A47A01F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA53B4B4-3945-401A-856B-DD34426D2F15}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="FlightsOnlyPositive" sheetId="1" r:id="rId1"/>
-    <sheet name="FlightsWithHotelsPositive" sheetId="2" r:id="rId2"/>
+    <sheet name="FlightsOnlyPositive" sheetId="3" r:id="rId1"/>
+    <sheet name="FlightsOnlyPosWAge" sheetId="1" r:id="rId2"/>
+    <sheet name="FlightsWithHotelsPositive" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="42">
   <si>
     <t>One-way</t>
   </si>
@@ -41,15 +42,9 @@
     <t>Mumbai</t>
   </si>
   <si>
-    <t>02/12/2019</t>
-  </si>
-  <si>
     <t>Departure Date (in dd/mm/yyyy)</t>
   </si>
   <si>
-    <t>12/01/2020</t>
-  </si>
-  <si>
     <t>Hotel Check-in Date (in dd/mm/yyyy)</t>
   </si>
   <si>
@@ -59,21 +54,9 @@
     <t>Hotel Check-out Date (in dd/mm/yyyy)</t>
   </si>
   <si>
-    <t>25/11/2019</t>
-  </si>
-  <si>
     <t>Washington</t>
   </si>
   <si>
-    <t>16/12/2019</t>
-  </si>
-  <si>
-    <t>17/12/2019</t>
-  </si>
-  <si>
-    <t>19/12/2019</t>
-  </si>
-  <si>
     <t>London</t>
   </si>
   <si>
@@ -86,15 +69,9 @@
     <t>Bengaluru</t>
   </si>
   <si>
-    <t>25/12/2019</t>
-  </si>
-  <si>
     <t>Trivandrum</t>
   </si>
   <si>
-    <t>18/12/2019</t>
-  </si>
-  <si>
     <t>new york</t>
   </si>
   <si>
@@ -108,29 +85,94 @@
   </si>
   <si>
     <t>Delhi</t>
-  </si>
-  <si>
-    <t>09/01/2020</t>
   </si>
   <si>
     <t>Instruction - Put the start tag (One-way) before the first column and the first row to be used and the end tag (One-way) after the last column and last row to be used.
 Only use future dates here.</t>
+  </si>
+  <si>
+    <t>AdultNos</t>
+  </si>
+  <si>
+    <t>ChildrenNos</t>
+  </si>
+  <si>
+    <t>InfantNos</t>
+  </si>
+  <si>
+    <t>ChildrenAges</t>
+  </si>
+  <si>
+    <t>InfantAges</t>
+  </si>
+  <si>
+    <t>Under1,1</t>
+  </si>
+  <si>
+    <t>2,4,8</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Instruction - Put the start tag (One-way) before the first column and the first row to be used and the end tag (One-way) after the last column and last row to be used.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Only use future dates here.</t>
+    </r>
+  </si>
+  <si>
+    <t>03/09/2020</t>
+  </si>
+  <si>
+    <t>07/12/2020</t>
+  </si>
+  <si>
+    <t>04/09/2020</t>
+  </si>
+  <si>
+    <t>06/09/2020</t>
+  </si>
+  <si>
+    <t>20 Sep 2020</t>
+  </si>
+  <si>
+    <t>OneWayAge</t>
+  </si>
+  <si>
+    <t>25 Sep 2020</t>
+  </si>
+  <si>
+    <t>01 Jan 2021</t>
+  </si>
+  <si>
+    <t>27 Dec 2020</t>
+  </si>
+  <si>
+    <t>19 Nov 2020</t>
+  </si>
+  <si>
+    <t>7 Jan 2021</t>
+  </si>
+  <si>
+    <t>12 Jan 2021</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
     </font>
     <font>
       <sz val="11"/>
@@ -149,6 +191,24 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Arial"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -176,12 +236,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -398,26 +460,178 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD5D1D3A-5071-4574-BCCD-29CCFD49D1EA}">
+  <dimension ref="A1:H6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="12.5" customWidth="1"/>
+    <col min="2" max="7" width="13.08203125" customWidth="1"/>
+    <col min="8" max="8" width="12.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="B2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="E2">
+        <v>2</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="B3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="E3">
+        <v>4</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="B4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="B5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="B6" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H1000"/>
+  <dimension ref="A1:J1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="7.6640625" customWidth="1"/>
+    <col min="1" max="1" width="11.6640625" customWidth="1"/>
     <col min="2" max="2" width="12.6640625" customWidth="1"/>
     <col min="3" max="3" width="15.6640625" customWidth="1"/>
     <col min="4" max="4" width="24.5" customWidth="1"/>
-    <col min="5" max="6" width="7.6640625" customWidth="1"/>
+    <col min="5" max="5" width="14.58203125" customWidth="1"/>
+    <col min="6" max="6" width="16.25" customWidth="1"/>
     <col min="7" max="7" width="24.4140625" customWidth="1"/>
     <col min="8" max="8" width="26.33203125" customWidth="1"/>
-    <col min="9" max="26" width="7.6640625" customWidth="1"/>
+    <col min="9" max="10" width="27.25" customWidth="1"/>
+    <col min="11" max="11" width="26.4140625" customWidth="1"/>
+    <col min="12" max="12" width="26" customWidth="1"/>
+    <col min="13" max="26" width="7.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>35</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>2</v>
@@ -428,84 +642,150 @@
       <c r="D1" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E1" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="17" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B2" s="1" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="E2">
+        <v>2</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="H2" t="s">
+        <v>28</v>
+      </c>
+      <c r="I2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="E3">
         <v>6</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="1" t="s">
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="G3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B4" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D3" s="3" t="s">
+      <c r="C4" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="D4" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="E4">
+        <v>4</v>
+      </c>
+      <c r="F4">
+        <v>2</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B5" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="D5" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B6" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="14" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="J7" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="49.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="I8" s="7" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D6" s="6" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="E7" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="9" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="10" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="11" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="12" spans="1:8" ht="31.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G12" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="H12" s="8"/>
-    </row>
-    <row r="13" spans="1:8" ht="46" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G13" s="8"/>
-      <c r="H13" s="8"/>
-    </row>
-    <row r="14" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="15" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="16" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+      <c r="J8" s="7"/>
+    </row>
+    <row r="9" spans="1:10" ht="27.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="I9" s="7"/>
+      <c r="J9" s="7"/>
+    </row>
+    <row r="10" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="11" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="12" spans="1:10" ht="31.5" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="13" spans="1:10" ht="46" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="14" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="15" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="16" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="17" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="18" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1492,32 +1772,35 @@
     <row r="1000" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="G12:H13"/>
+    <mergeCell ref="I8:J9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="portrait"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:J12"/>
+  <dimension ref="A1:H12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="4" max="4" width="31.4140625" customWidth="1"/>
     <col min="5" max="5" width="29" customWidth="1"/>
     <col min="6" max="6" width="28.6640625" customWidth="1"/>
+    <col min="8" max="8" width="25.5" customWidth="1"/>
     <col min="9" max="9" width="19.83203125" customWidth="1"/>
     <col min="10" max="10" width="18.9140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
@@ -1527,87 +1810,86 @@
       <c r="C1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="F1" s="4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" ht="14.5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="2" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
       <c r="B2" s="2" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" ht="14.5" x14ac:dyDescent="0.35">
+        <v>30</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
       <c r="B3" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="F3" s="7" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" ht="14.5" x14ac:dyDescent="0.35">
+        <v>31</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
       <c r="B4" s="2" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="F4" s="7" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="G5" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" ht="49.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="I11" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="J11" s="8"/>
-    </row>
-    <row r="12" spans="1:10" ht="34" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="I12" s="8"/>
-      <c r="J12" s="8"/>
+        <v>19</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="14" x14ac:dyDescent="0.3"/>
+    <row r="11" spans="1:8" ht="49.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G11" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="H11" s="7"/>
+    </row>
+    <row r="12" spans="1:8" ht="34" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G12" s="7"/>
+      <c r="H12" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="I11:J12"/>
+    <mergeCell ref="G11:H12"/>
   </mergeCells>
-  <phoneticPr fontId="4" type="noConversion"/>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Added new DataProviders, rearranged and added some more test methods.
</commit_message>
<xml_diff>
--- a/Expedia_automation/Data_sheets/Data_sheets_expedia.xlsx
+++ b/Expedia_automation/Data_sheets/Data_sheets_expedia.xlsx
@@ -8,24 +8,23 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Selenium\Selenium projects\Expedia_automation\Data_sheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA53B4B4-3945-401A-856B-DD34426D2F15}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11C14C94-748E-4C80-9385-479CDAD158C9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="FlightsOnlyPositive" sheetId="3" r:id="rId1"/>
-    <sheet name="FlightsOnlyPosWAge" sheetId="1" r:id="rId2"/>
-    <sheet name="FlightsWithHotelsPositive" sheetId="2" r:id="rId3"/>
+    <sheet name="OneWayFlightsPosTravellers" sheetId="3" r:id="rId1"/>
+    <sheet name="OneWayFlightsPosDefaultDate" sheetId="4" r:id="rId2"/>
+    <sheet name="OneWayFlightsPosDate" sheetId="5" r:id="rId3"/>
+    <sheet name="FlightsOnlyPosWAge" sheetId="1" r:id="rId4"/>
+    <sheet name="FlightsWithHotelsPositive" sheetId="2" r:id="rId5"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="42">
-  <si>
-    <t>One-way</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="47">
   <si>
     <t>OneWayHotels</t>
   </si>
@@ -162,6 +161,24 @@
   </si>
   <si>
     <t>12 Jan 2021</t>
+  </si>
+  <si>
+    <t>OneWayFlightsTravellers</t>
+  </si>
+  <si>
+    <t>Kozhikode</t>
+  </si>
+  <si>
+    <t>Dubai</t>
+  </si>
+  <si>
+    <t>OneWayFlightsPos</t>
+  </si>
+  <si>
+    <t>OneWayFlightsPosDate</t>
+  </si>
+  <si>
+    <t>Date</t>
   </si>
 </sst>
 </file>
@@ -463,141 +480,237 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD5D1D3A-5071-4574-BCCD-29CCFD49D1EA}">
   <dimension ref="A1:H6"/>
   <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="24.33203125" customWidth="1"/>
+    <col min="2" max="7" width="13.08203125" customWidth="1"/>
+    <col min="8" max="8" width="22.4140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="B2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="E2">
+        <v>2</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="B3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="E3">
+        <v>4</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="B4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="B5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="B6" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA583240-635E-4608-A31D-5DD5BA037B77}">
+  <dimension ref="A1:D3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="19.58203125" customWidth="1"/>
+    <col min="2" max="2" width="12.08203125" customWidth="1"/>
+    <col min="3" max="3" width="17.33203125" customWidth="1"/>
+    <col min="4" max="4" width="16.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A0505F9-B8CF-4B2F-A121-89B24FCC7D64}">
+  <dimension ref="A1:E3"/>
+  <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.5" customWidth="1"/>
-    <col min="2" max="7" width="13.08203125" customWidth="1"/>
-    <col min="8" max="8" width="12.83203125" customWidth="1"/>
+    <col min="1" max="1" width="22.9140625" customWidth="1"/>
+    <col min="2" max="2" width="12" customWidth="1"/>
+    <col min="3" max="4" width="14.33203125" customWidth="1"/>
+    <col min="5" max="5" width="23.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
+    <row r="1" spans="1:5" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>45</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>3</v>
-      </c>
       <c r="D1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="B2" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>5</v>
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="B2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C2" t="s">
+        <v>43</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="E2">
-        <v>2</v>
-      </c>
-      <c r="F2">
-        <v>1</v>
-      </c>
-      <c r="G2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="B3" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="E3">
-        <v>4</v>
-      </c>
-      <c r="F3">
-        <v>1</v>
-      </c>
-      <c r="G3">
-        <v>0</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="B4" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="E4">
-        <v>1</v>
-      </c>
-      <c r="F4">
-        <v>1</v>
-      </c>
-      <c r="G4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="B5" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="E5">
-        <v>1</v>
-      </c>
-      <c r="F5">
-        <v>0</v>
-      </c>
-      <c r="G5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="B6" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D6" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="E6">
-        <v>1</v>
-      </c>
-      <c r="F6">
-        <v>0</v>
-      </c>
-      <c r="G6">
-        <v>0</v>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E3" t="s">
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -605,7 +718,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J1000"/>
   <sheetViews>
@@ -631,42 +744,42 @@
   <sheetData>
     <row r="1" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>4</v>
-      </c>
       <c r="E1" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>25</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="17" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B2" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E2">
         <v>2</v>
@@ -678,21 +791,21 @@
         <v>1</v>
       </c>
       <c r="H2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B3" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E3">
         <v>6</v>
@@ -706,13 +819,13 @@
     </row>
     <row r="4" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B4" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E4">
         <v>4</v>
@@ -726,13 +839,13 @@
     </row>
     <row r="5" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B5" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E5">
         <v>1</v>
@@ -746,13 +859,13 @@
     </row>
     <row r="6" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B6" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E6">
         <v>1</v>
@@ -766,12 +879,12 @@
     </row>
     <row r="7" spans="1:10" ht="14" customHeight="1" x14ac:dyDescent="0.35">
       <c r="J7" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="49.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="I8" s="7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="J8" s="7"/>
     </row>
@@ -1779,7 +1892,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -1802,82 +1915,82 @@
   <sheetData>
     <row r="1" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>3</v>
-      </c>
       <c r="D1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="2" t="s">
-        <v>7</v>
-      </c>
       <c r="F1" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
       <c r="B2" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E2" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="F2" s="5" t="s">
         <v>32</v>
-      </c>
-      <c r="F2" s="5" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
       <c r="B3" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D3" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="E3" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="E3" s="5" t="s">
-        <v>32</v>
-      </c>
       <c r="F3" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
       <c r="B4" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="14" x14ac:dyDescent="0.3"/>
     <row r="11" spans="1:8" ht="49.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="G11" s="8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H11" s="7"/>
     </row>

</xml_diff>

<commit_message>
Created CustomDriver class, modified data sheet & FlightsOneWay
CustomDriver class will contain common WebDriver functions and page
classes will inherit it and call its methods eventually.
</commit_message>
<xml_diff>
--- a/Expedia_automation/Data_sheets/Data_sheets_expedia.xlsx
+++ b/Expedia_automation/Data_sheets/Data_sheets_expedia.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Selenium\Selenium projects\Expedia_automation\Data_sheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11C14C94-748E-4C80-9385-479CDAD158C9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27AC57E6-89CB-4BBB-8AB0-475C0471472A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -672,7 +672,7 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Designed a date providing code and fixed some other code issues.
</commit_message>
<xml_diff>
--- a/Expedia_automation/Data_sheets/Data_sheets_expedia.xlsx
+++ b/Expedia_automation/Data_sheets/Data_sheets_expedia.xlsx
@@ -1,30 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Selenium\Selenium projects\Expedia_automation\Data_sheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27AC57E6-89CB-4BBB-8AB0-475C0471472A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A33914EB-512A-4598-BF26-1DEF53CC95EA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="OneWayFlightsPosTravellers" sheetId="3" r:id="rId1"/>
-    <sheet name="OneWayFlightsPosDefaultDate" sheetId="4" r:id="rId2"/>
-    <sheet name="OneWayFlightsPosDate" sheetId="5" r:id="rId3"/>
-    <sheet name="FlightsOnlyPosWAge" sheetId="1" r:id="rId4"/>
-    <sheet name="FlightsWithHotelsPositive" sheetId="2" r:id="rId5"/>
+    <sheet name="Important Information" sheetId="6" r:id="rId1"/>
+    <sheet name="OneWayFlightsPosTravellers" sheetId="3" r:id="rId2"/>
+    <sheet name="OneWayFlightsPosDefaultDate" sheetId="4" r:id="rId3"/>
+    <sheet name="OneWayFlightsPosDate" sheetId="5" r:id="rId4"/>
+    <sheet name="FlightsOnlyPosWAge" sheetId="1" r:id="rId5"/>
+    <sheet name="FlightsWithHotelsPositive" sheetId="2" r:id="rId6"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="62">
   <si>
     <t>OneWayHotels</t>
   </si>
@@ -179,6 +180,63 @@
   </si>
   <si>
     <t>Date</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">All sheets with the word 'Pos' within their tab name indicate test data for positive test cases. If one of the columns in any of those sheets contains date, ensure to provide only current or future dates. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Don't provide past dates else the test will fail.</t>
+    </r>
+  </si>
+  <si>
+    <t>Hyderabad</t>
+  </si>
+  <si>
+    <t>New Delhi</t>
+  </si>
+  <si>
+    <t>Bangkok</t>
+  </si>
+  <si>
+    <t>Kolkata</t>
+  </si>
+  <si>
+    <t>Tokyo</t>
+  </si>
+  <si>
+    <t>Chicago</t>
+  </si>
+  <si>
+    <t>Bangalore</t>
+  </si>
+  <si>
+    <t>Bombay</t>
+  </si>
+  <si>
+    <t>15 Feb 2021</t>
+  </si>
+  <si>
+    <t>Bhubaneswar</t>
+  </si>
+  <si>
+    <t>6 Jun 2021</t>
+  </si>
+  <si>
+    <t>3 May 2021</t>
+  </si>
+  <si>
+    <t>6 Feb 2021</t>
+  </si>
+  <si>
+    <t>10 Feb 2021</t>
   </si>
 </sst>
 </file>
@@ -249,7 +307,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -257,6 +315,13 @@
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -477,6 +542,54 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03D385C2-6E58-432F-BCCC-55E697E10F02}">
+  <dimension ref="A1:A8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:A8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="42.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1" s="8" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" s="9"/>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A3" s="9"/>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A4" s="9"/>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A5" s="9"/>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A6" s="9"/>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A7" s="9"/>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A8" s="9"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:A8"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD5D1D3A-5071-4574-BCCD-29CCFD49D1EA}">
   <dimension ref="A1:H6"/>
   <sheetViews>
@@ -622,12 +735,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA583240-635E-4608-A31D-5DD5BA037B77}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:D3"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -658,7 +771,31 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="D3" t="s">
+      <c r="B3" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B4" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B5" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D6" t="s">
         <v>44</v>
       </c>
     </row>
@@ -667,13 +804,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A0505F9-B8CF-4B2F-A121-89B24FCC7D64}">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
@@ -705,11 +840,55 @@
         <v>43</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="E3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="B3" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="B4" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="B5" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="B6" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E7" t="s">
         <v>45</v>
       </c>
     </row>
@@ -718,7 +897,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J1000"/>
   <sheetViews>
@@ -883,14 +1062,14 @@
       </c>
     </row>
     <row r="8" spans="1:10" ht="49.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="I8" s="7" t="s">
+      <c r="I8" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="J8" s="7"/>
+      <c r="J8" s="10"/>
     </row>
     <row r="9" spans="1:10" ht="27.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="I9" s="7"/>
-      <c r="J9" s="7"/>
+      <c r="I9" s="10"/>
+      <c r="J9" s="10"/>
     </row>
     <row r="10" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="11" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1892,7 +2071,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -1989,14 +2168,14 @@
     </row>
     <row r="5" spans="1:8" ht="14" x14ac:dyDescent="0.3"/>
     <row r="11" spans="1:8" ht="49.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G11" s="8" t="s">
+      <c r="G11" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="H11" s="7"/>
+      <c r="H11" s="10"/>
     </row>
     <row r="12" spans="1:8" ht="34" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G12" s="7"/>
-      <c r="H12" s="7"/>
+      <c r="G12" s="10"/>
+      <c r="H12" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Included driver in the project and modified gitignore
</commit_message>
<xml_diff>
--- a/Expedia_automation/Data_sheets/Data_sheets_expedia.xlsx
+++ b/Expedia_automation/Data_sheets/Data_sheets_expedia.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Selenium\Selenium projects\Expedia_automation\Data_sheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A33914EB-512A-4598-BF26-1DEF53CC95EA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69DBE30A-916A-4CE4-8D54-BAEFC735D5B6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -221,9 +221,6 @@
     <t>Bombay</t>
   </si>
   <si>
-    <t>15 Feb 2021</t>
-  </si>
-  <si>
     <t>Bhubaneswar</t>
   </si>
   <si>
@@ -233,10 +230,13 @@
     <t>3 May 2021</t>
   </si>
   <si>
-    <t>6 Feb 2021</t>
-  </si>
-  <si>
-    <t>10 Feb 2021</t>
+    <t>20 Feb 2021</t>
+  </si>
+  <si>
+    <t>25 Feb 2021</t>
+  </si>
+  <si>
+    <t>7 Mar 2021</t>
   </si>
 </sst>
 </file>
@@ -808,7 +808,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A0505F9-B8CF-4B2F-A121-89B24FCC7D64}">
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
@@ -840,7 +842,7 @@
         <v>43</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="14.5" x14ac:dyDescent="0.35">
@@ -851,7 +853,7 @@
         <v>14</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="14.5" x14ac:dyDescent="0.35">
@@ -862,7 +864,7 @@
         <v>53</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="14.5" x14ac:dyDescent="0.35">
@@ -873,18 +875,18 @@
         <v>55</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="14.5" x14ac:dyDescent="0.35">
       <c r="B6" s="7" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C6" s="7" t="s">
         <v>19</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Made some debugging in the POM file.
</commit_message>
<xml_diff>
--- a/Expedia_automation/Data_sheets/Data_sheets_expedia.xlsx
+++ b/Expedia_automation/Data_sheets/Data_sheets_expedia.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Selenium\Selenium projects\Expedia_automation\Data_sheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69DBE30A-916A-4CE4-8D54-BAEFC735D5B6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{869A225A-D619-491E-95B3-F84D817323F9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Important Information" sheetId="6" r:id="rId1"/>
@@ -739,7 +739,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA583240-635E-4608-A31D-5DD5BA037B77}">
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
@@ -808,9 +808,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A0505F9-B8CF-4B2F-A121-89B24FCC7D64}">
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>

</xml_diff>